<commit_message>
post jhou meeting files
</commit_message>
<xml_diff>
--- a/Bonnie's Codes/CREATE/runway_c01_16_missingraw.xlsx
+++ b/Bonnie's Codes/CREATE/runway_c01_16_missingraw.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve">labanimalid</t>
   </si>
@@ -156,153 +156,6 @@
   </si>
   <si>
     <t xml:space="preserve">U706</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U713</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U714</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U715</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U716</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U717</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U718</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U719</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U720</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U721</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U722</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U723</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U724</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U725</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U726</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U727</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U728</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U729</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U731</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U732</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U733</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U734</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U735</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U736</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U737</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U738</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U739</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U740</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U741</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U742</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U743</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U744</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U745</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U746</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U747</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U748</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U749</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U750</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U751</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U752</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U753</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U754</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U755</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U756</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U757</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U758</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U759</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U760</t>
   </si>
 </sst>
 </file>
@@ -930,486 +783,6 @@
       <c r="C27"/>
       <c r="D27"/>
     </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28"/>
-      <c r="D28"/>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29"/>
-      <c r="D29"/>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30"/>
-      <c r="D30"/>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31"/>
-      <c r="D31"/>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32"/>
-      <c r="D32"/>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33"/>
-      <c r="D33"/>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34"/>
-      <c r="D34"/>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35"/>
-      <c r="D35"/>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>57</v>
-      </c>
-      <c r="B36" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36"/>
-      <c r="D36"/>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37"/>
-      <c r="D37"/>
-    </row>
-    <row r="38">
-      <c r="A38" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38"/>
-      <c r="D38"/>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>60</v>
-      </c>
-      <c r="B39" t="s">
-        <v>49</v>
-      </c>
-      <c r="C39"/>
-      <c r="D39"/>
-    </row>
-    <row r="40">
-      <c r="A40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B40" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40"/>
-      <c r="D40"/>
-    </row>
-    <row r="41">
-      <c r="A41" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C41"/>
-      <c r="D41"/>
-    </row>
-    <row r="42">
-      <c r="A42" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" t="s">
-        <v>49</v>
-      </c>
-      <c r="C42"/>
-      <c r="D42"/>
-    </row>
-    <row r="43">
-      <c r="A43" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43"/>
-      <c r="D43"/>
-    </row>
-    <row r="44">
-      <c r="A44" t="s">
-        <v>65</v>
-      </c>
-      <c r="B44" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44"/>
-      <c r="D44"/>
-    </row>
-    <row r="45">
-      <c r="A45" t="s">
-        <v>66</v>
-      </c>
-      <c r="B45" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45"/>
-      <c r="D45"/>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>67</v>
-      </c>
-      <c r="B46" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46"/>
-      <c r="D46"/>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>68</v>
-      </c>
-      <c r="B47" t="s">
-        <v>49</v>
-      </c>
-      <c r="C47"/>
-      <c r="D47"/>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
-        <v>69</v>
-      </c>
-      <c r="B48" t="s">
-        <v>49</v>
-      </c>
-      <c r="C48"/>
-      <c r="D48"/>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>70</v>
-      </c>
-      <c r="B49" t="s">
-        <v>49</v>
-      </c>
-      <c r="C49"/>
-      <c r="D49"/>
-    </row>
-    <row r="50">
-      <c r="A50" t="s">
-        <v>71</v>
-      </c>
-      <c r="B50" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50"/>
-      <c r="D50"/>
-    </row>
-    <row r="51">
-      <c r="A51" t="s">
-        <v>72</v>
-      </c>
-      <c r="B51" t="s">
-        <v>49</v>
-      </c>
-      <c r="C51"/>
-      <c r="D51"/>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
-        <v>73</v>
-      </c>
-      <c r="B52" t="s">
-        <v>49</v>
-      </c>
-      <c r="C52"/>
-      <c r="D52"/>
-    </row>
-    <row r="53">
-      <c r="A53" t="s">
-        <v>74</v>
-      </c>
-      <c r="B53" t="s">
-        <v>49</v>
-      </c>
-      <c r="C53"/>
-      <c r="D53"/>
-    </row>
-    <row r="54">
-      <c r="A54" t="s">
-        <v>75</v>
-      </c>
-      <c r="B54" t="s">
-        <v>49</v>
-      </c>
-      <c r="C54"/>
-      <c r="D54"/>
-    </row>
-    <row r="55">
-      <c r="A55" t="s">
-        <v>76</v>
-      </c>
-      <c r="B55" t="s">
-        <v>49</v>
-      </c>
-      <c r="C55"/>
-      <c r="D55"/>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
-        <v>77</v>
-      </c>
-      <c r="B56" t="s">
-        <v>49</v>
-      </c>
-      <c r="C56"/>
-      <c r="D56"/>
-    </row>
-    <row r="57">
-      <c r="A57" t="s">
-        <v>78</v>
-      </c>
-      <c r="B57" t="s">
-        <v>49</v>
-      </c>
-      <c r="C57"/>
-      <c r="D57"/>
-    </row>
-    <row r="58">
-      <c r="A58" t="s">
-        <v>79</v>
-      </c>
-      <c r="B58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C58"/>
-      <c r="D58"/>
-    </row>
-    <row r="59">
-      <c r="A59" t="s">
-        <v>80</v>
-      </c>
-      <c r="B59" t="s">
-        <v>49</v>
-      </c>
-      <c r="C59"/>
-      <c r="D59"/>
-    </row>
-    <row r="60">
-      <c r="A60" t="s">
-        <v>81</v>
-      </c>
-      <c r="B60" t="s">
-        <v>49</v>
-      </c>
-      <c r="C60"/>
-      <c r="D60"/>
-    </row>
-    <row r="61">
-      <c r="A61" t="s">
-        <v>82</v>
-      </c>
-      <c r="B61" t="s">
-        <v>49</v>
-      </c>
-      <c r="C61"/>
-      <c r="D61"/>
-    </row>
-    <row r="62">
-      <c r="A62" t="s">
-        <v>83</v>
-      </c>
-      <c r="B62" t="s">
-        <v>49</v>
-      </c>
-      <c r="C62"/>
-      <c r="D62"/>
-    </row>
-    <row r="63">
-      <c r="A63" t="s">
-        <v>84</v>
-      </c>
-      <c r="B63" t="s">
-        <v>49</v>
-      </c>
-      <c r="C63"/>
-      <c r="D63"/>
-    </row>
-    <row r="64">
-      <c r="A64" t="s">
-        <v>85</v>
-      </c>
-      <c r="B64" t="s">
-        <v>49</v>
-      </c>
-      <c r="C64"/>
-      <c r="D64"/>
-    </row>
-    <row r="65">
-      <c r="A65" t="s">
-        <v>86</v>
-      </c>
-      <c r="B65" t="s">
-        <v>49</v>
-      </c>
-      <c r="C65"/>
-      <c r="D65"/>
-    </row>
-    <row r="66">
-      <c r="A66" t="s">
-        <v>87</v>
-      </c>
-      <c r="B66" t="s">
-        <v>49</v>
-      </c>
-      <c r="C66"/>
-      <c r="D66"/>
-    </row>
-    <row r="67">
-      <c r="A67" t="s">
-        <v>88</v>
-      </c>
-      <c r="B67" t="s">
-        <v>49</v>
-      </c>
-      <c r="C67"/>
-      <c r="D67"/>
-    </row>
-    <row r="68">
-      <c r="A68" t="s">
-        <v>89</v>
-      </c>
-      <c r="B68" t="s">
-        <v>49</v>
-      </c>
-      <c r="C68"/>
-      <c r="D68"/>
-    </row>
-    <row r="69">
-      <c r="A69" t="s">
-        <v>90</v>
-      </c>
-      <c r="B69" t="s">
-        <v>49</v>
-      </c>
-      <c r="C69"/>
-      <c r="D69"/>
-    </row>
-    <row r="70">
-      <c r="A70" t="s">
-        <v>91</v>
-      </c>
-      <c r="B70" t="s">
-        <v>49</v>
-      </c>
-      <c r="C70"/>
-      <c r="D70"/>
-    </row>
-    <row r="71">
-      <c r="A71" t="s">
-        <v>92</v>
-      </c>
-      <c r="B71" t="s">
-        <v>49</v>
-      </c>
-      <c r="C71"/>
-      <c r="D71"/>
-    </row>
-    <row r="72">
-      <c r="A72" t="s">
-        <v>93</v>
-      </c>
-      <c r="B72" t="s">
-        <v>49</v>
-      </c>
-      <c r="C72"/>
-      <c r="D72"/>
-    </row>
-    <row r="73">
-      <c r="A73" t="s">
-        <v>94</v>
-      </c>
-      <c r="B73" t="s">
-        <v>49</v>
-      </c>
-      <c r="C73"/>
-      <c r="D73"/>
-    </row>
-    <row r="74">
-      <c r="A74" t="s">
-        <v>95</v>
-      </c>
-      <c r="B74" t="s">
-        <v>49</v>
-      </c>
-      <c r="C74"/>
-      <c r="D74"/>
-    </row>
-    <row r="75">
-      <c r="A75" t="s">
-        <v>96</v>
-      </c>
-      <c r="B75" t="s">
-        <v>49</v>
-      </c>
-      <c r="C75"/>
-      <c r="D75"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>